<commit_message>
Continued work on Assignment 3
</commit_message>
<xml_diff>
--- a/Assignment 3/Assignment3.xlsx
+++ b/Assignment 3/Assignment3.xlsx
@@ -8,14 +8,52 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59a73ea97849167b/Documents/GitHub/Decision-Making-and-Problem-Solving-course-2021/Assignment 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC104849095D54725ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4743905-FB67-42E5-9084-CACA1F58F5D0}"/>
+  <xr:revisionPtr revIDLastSave="987" documentId="11_F25DC773A252ABDACC104849095D54725ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CC709B4-E9DF-4024-BAF5-37CED0647132}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
     <sheet name="3" sheetId="2" r:id="rId2"/>
+    <sheet name="5" sheetId="3" r:id="rId3"/>
+    <sheet name="6" sheetId="4" r:id="rId4"/>
+    <sheet name="7" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'7'!$B$15:$B$24</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'7'!$B$15:$B$24</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'7'!$F$15</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'7'!$D$15</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'7'!$H$15</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -57,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t>Site</t>
   </si>
@@ -135,6 +173,63 @@
   </si>
   <si>
     <t>v9</t>
+  </si>
+  <si>
+    <t>w1</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>w3</t>
+  </si>
+  <si>
+    <t>w4</t>
+  </si>
+  <si>
+    <t>w5</t>
+  </si>
+  <si>
+    <t>w6</t>
+  </si>
+  <si>
+    <t>w7</t>
+  </si>
+  <si>
+    <t>w8</t>
+  </si>
+  <si>
+    <t>w9</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Normalizied value</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>V'</t>
+  </si>
+  <si>
+    <t>V'/V</t>
+  </si>
+  <si>
+    <t>Objective function</t>
+  </si>
+  <si>
+    <t>Sites in use</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>=&lt;</t>
+  </si>
+  <si>
+    <t>Variables</t>
   </si>
 </sst>
 </file>
@@ -214,12 +309,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,6 +350,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fi-FI"/>
+              <a:t>v</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-FI"/>
+              <a:t>2</a:t>
+            </a:r>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2409,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3229,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183EEB28-5970-46F2-8D62-7C404E2AFE6A}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3302,7 +3430,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <f>IF(F4&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F4)),0)</f>
+        <f t="shared" ref="G4:G14" si="1">IF(F4&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F4)),0)</f>
         <v>0</v>
       </c>
       <c r="J4" cm="1">
@@ -3326,7 +3454,7 @@
         <v>2.7</v>
       </c>
       <c r="G5">
-        <f>IF(F5&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F5)),0)</f>
+        <f t="shared" si="1"/>
         <v>4.7991587687201055E-2</v>
       </c>
     </row>
@@ -3343,7 +3471,7 @@
         <v>2.4</v>
       </c>
       <c r="G6">
-        <f>IF(F6&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F6)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.10343646283322631</v>
       </c>
     </row>
@@ -3360,7 +3488,7 @@
         <v>2.1</v>
       </c>
       <c r="G7">
-        <f>IF(F7&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F7)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.16749215109248683</v>
       </c>
     </row>
@@ -3377,7 +3505,7 @@
         <v>1.7999999999999998</v>
       </c>
       <c r="G8">
-        <f>IF(F8&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F8)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.24149594653004816</v>
       </c>
     </row>
@@ -3394,7 +3522,7 @@
         <v>1.5</v>
       </c>
       <c r="G9">
-        <f>IF(F9&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F9)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.3269928303820871</v>
       </c>
     </row>
@@ -3411,7 +3539,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="G10">
-        <f>IF(F10&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F10)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.42576772571264371</v>
       </c>
     </row>
@@ -3428,7 +3556,7 @@
         <v>0.90000000000000036</v>
       </c>
       <c r="G11">
-        <f>IF(F11&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F11)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.53988276134887792</v>
       </c>
     </row>
@@ -3445,7 +3573,7 @@
         <v>0.59999999999999964</v>
       </c>
       <c r="G12">
-        <f>IF(F12&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F12)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.67172032305602292</v>
       </c>
     </row>
@@ -3462,7 +3590,7 @@
         <v>0.29999999999999982</v>
       </c>
       <c r="G13">
-        <f>IF(F13&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F13)),0)</f>
+        <f t="shared" si="1"/>
         <v>0.82403279073373781</v>
       </c>
     </row>
@@ -3479,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IF(F14&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-F14)),0)</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
@@ -3487,4 +3615,2143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00685FA3-0948-4D0F-8D04-8A09FCDF86F3}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6">
+        <v>6.2130999999999999E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="6">
+        <f>E2*($B$2*'2'!E2+$B$3*'2'!G2+$B$4*'2'!I2+$B$5*'2'!K2+$B$6*'2'!M2+$B$7*'2'!O2+$B$8*'2'!Q2+$B$9*'2'!S2+$B$10*'2'!U2)</f>
+        <v>0.25628489290043294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6">
+        <v>4.1202700000000002E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <f>E3*($B$2*'2'!E3+$B$3*'2'!G3+$B$4*'2'!I3+$B$5*'2'!K3+$B$6*'2'!M3+$B$7*'2'!O3+$B$8*'2'!Q3+$B$9*'2'!S3+$B$10*'2'!U3)</f>
+        <v>0.8788362408369409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2.74685E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="F4" s="6">
+        <f>E4*($B$2*'2'!E4+$B$3*'2'!G4+$B$4*'2'!I4+$B$5*'2'!K4+$B$6*'2'!M4+$B$7*'2'!O4+$B$8*'2'!Q4+$B$9*'2'!S4+$B$10*'2'!U4)</f>
+        <v>0.70918390614498517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="6">
+        <v>7.6779E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <f>E5*($B$2*'2'!E5+$B$3*'2'!G5+$B$4*'2'!I5+$B$5*'2'!K5+$B$6*'2'!M5+$B$7*'2'!O5+$B$8*'2'!Q5+$B$9*'2'!S5+$B$10*'2'!U5)</f>
+        <v>0.64160641702378807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.102372</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="6">
+        <f>E6*($B$2*'2'!E6+$B$3*'2'!G6+$B$4*'2'!I6+$B$5*'2'!K6+$B$6*'2'!M6+$B$7*'2'!O6+$B$8*'2'!Q6+$B$9*'2'!S6+$B$10*'2'!U6)</f>
+        <v>0.25058569968253969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.11516800000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <f>E7*($B$2*'2'!E7+$B$3*'2'!G7+$B$4*'2'!I7+$B$5*'2'!K7+$B$6*'2'!M7+$B$7*'2'!O7+$B$8*'2'!Q7+$B$9*'2'!S7+$B$10*'2'!U7)</f>
+        <v>0.69852150562770565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.42654999999999998</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6">
+        <f>E8*($B$2*'2'!E8+$B$3*'2'!G8+$B$4*'2'!I8+$B$5*'2'!K8+$B$6*'2'!M8+$B$7*'2'!O8+$B$8*'2'!Q8+$B$9*'2'!S8+$B$10*'2'!U8)</f>
+        <v>0.69698269940094792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6.8181400000000003E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="6">
+        <f>E9*($B$2*'2'!E9+$B$3*'2'!G9+$B$4*'2'!I9+$B$5*'2'!K9+$B$6*'2'!M9+$B$7*'2'!O9+$B$8*'2'!Q9+$B$9*'2'!S9+$B$10*'2'!U9)</f>
+        <v>0.23132703541558444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6">
+        <v>8.0146999999999996E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <f>E10*($B$2*'2'!E10+$B$3*'2'!G10+$B$4*'2'!I10+$B$5*'2'!K10+$B$6*'2'!M10+$B$7*'2'!O10+$B$8*'2'!Q10+$B$9*'2'!S10+$B$10*'2'!U10)</f>
+        <v>0.3718140746746032</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="F11" s="6">
+        <f>E11*($B$2*'2'!E11+$B$3*'2'!G11+$B$4*'2'!I11+$B$5*'2'!K11+$B$6*'2'!M11+$B$7*'2'!O11+$B$8*'2'!Q11+$B$9*'2'!S11+$B$10*'2'!U11)</f>
+        <v>0.4835755523448978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB92054-4C8A-4904-A0BD-9130A64C4106}">
+  <dimension ref="A1:W22"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2400</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <f>1/40*D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" ref="G2:G10" si="0">IF(F2&lt;2,0,IF(F2&lt;6,1/12*F2-1/6,IF(F2&lt;15,1/27*F2+1/9,IF(F2&lt;=30,1/45*F2+1/3,1))))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="H2" s="2">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2:I10" si="1">IF(H2&lt;2,0,IF(H2&lt;9,1/14*H2-1/7,IF(H2&lt;30,1/42*H2+2/7,1)))</f>
+        <v>0.59523809523809523</v>
+      </c>
+      <c r="J2" s="2">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3">
+        <f>1/18*J2-1/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="L2" s="2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3">
+        <f>1/20*L2</f>
+        <v>0.2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3">
+        <f>1/20*N2</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>1/40*P2</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3">
+        <f>IF(R2&lt;10,1024/1023*(1-2^(-R2)),1)</f>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T2" s="2">
+        <v>4</v>
+      </c>
+      <c r="U2" s="3">
+        <f>IF(T2&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-T2)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <f>C2*($B$14*E2+$B$15*G2+$B$16*I2+$B$17*K2+$B$18*M2+$B$19*O2+$B$20*Q2+$B$21*S2+$B$22*U2)</f>
+        <v>0.34443709893310992</v>
+      </c>
+      <c r="W2" s="6" cm="1">
+        <f t="array" ref="W2:W11">V2:V11/'5'!F2:F11</f>
+        <v>1.3439617725221293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5700</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E11" si="2">1/40*D3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F3" s="2">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K11" si="3">1/18*J3-1/9</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M11" si="4">1/20*L3</f>
+        <v>0.75</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" ref="O3:O11" si="5">1/20*N3</f>
+        <v>0.25</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q11" si="6">1/40*P3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S11" si="7">IF(R3&lt;10,1024/1023*(1-2^(-R3)),1)</f>
+        <v>0.75073313782991202</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" ref="U3:U11" si="8">IF(T3&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-T3)),0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="V3" s="6">
+        <f t="shared" ref="V3:V11" si="9">C3*($B$14*E3+$B$15*G3+$B$16*I3+$B$17*K3+$B$18*M3+$B$19*O3+$B$20*Q3+$B$21*S3+$B$22*U3)</f>
+        <v>1.1811202225070987</v>
+      </c>
+      <c r="W3" s="6">
+        <v>1.3439593949633712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4725</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="8"/>
+        <v>0.5817316552559979</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" si="9"/>
+        <v>0.95311641287991355</v>
+      </c>
+      <c r="W4" s="6">
+        <v>1.3439622707471015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7800</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="F5" s="2">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>17</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="4"/>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="8"/>
+        <v>0.42576772571264371</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="9"/>
+        <v>0.8622932515650924</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1.3439598306466474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1560</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H6" s="2">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="J6" s="2">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>16</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="P6" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="6"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="9"/>
+        <v>0.33677718806349211</v>
+      </c>
+      <c r="W6" s="6">
+        <v>1.3439601241816517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4500</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>24</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>19</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="N7" s="2">
+        <v>16</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="8"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="V7" s="6">
+        <f t="shared" si="9"/>
+        <v>0.93878600139645307</v>
+      </c>
+      <c r="W7" s="6">
+        <v>1.3439614869879215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6150</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>9</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N8" s="2">
+        <v>10</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>9</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.99902248289345064</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="8"/>
+        <v>0.1909830056250526</v>
+      </c>
+      <c r="V8" s="6">
+        <f t="shared" si="9"/>
+        <v>0.93671765192861756</v>
+      </c>
+      <c r="W8" s="6">
+        <v>1.3439611237606333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1728</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="1"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L9" s="2">
+        <v>8</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>10</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="T9" s="2">
+        <v>4</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="6">
+        <f t="shared" si="9"/>
+        <v>0.31089460375324679</v>
+      </c>
+      <c r="W9" s="6">
+        <v>1.3439613886665576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1859</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="F10" s="2">
+        <v>29</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="H10" s="2">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="J10" s="2">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666652</v>
+      </c>
+      <c r="L10" s="2">
+        <v>8</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>16</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="P10" s="2">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>10</v>
+      </c>
+      <c r="U10" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <f t="shared" si="9"/>
+        <v>0.49970376936507938</v>
+      </c>
+      <c r="W10" s="6">
+        <v>1.3439614135166886</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4800</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F11" s="2">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4">
+        <f>IF(F11&lt;2,0,IF(F11&lt;6,1/12*F11-1/6,IF(F11&lt;15,1/27*F11+1/9,IF(F11&lt;=30,1/45*F11+1/3,1))))</f>
+        <v>0.62962962962962954</v>
+      </c>
+      <c r="H11" s="2">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4">
+        <f>IF(H11&lt;2,0,IF(H11&lt;9,1/14*H11-1/7,IF(H11&lt;30,1/42*H11+2/7,1)))</f>
+        <v>0.80952380952380942</v>
+      </c>
+      <c r="J11" s="2">
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+      <c r="S11" s="3">
+        <f t="shared" si="7"/>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="U11" s="3">
+        <f t="shared" si="8"/>
+        <v>0.67172032305602269</v>
+      </c>
+      <c r="V11" s="6">
+        <f t="shared" si="9"/>
+        <v>0.64990553645513494</v>
+      </c>
+      <c r="W11" s="6">
+        <v>1.3439586292228574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6">
+        <v>8.3501599999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6">
+        <v>5.5374699999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3.6916499999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.103188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.13758400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.154782</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.22930600000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>9.1633000000000006E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.107714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CEF85D-FCC4-425E-B48B-994A35BB5B53}">
+  <dimension ref="A1:V24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2400</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <f>1/40*D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" ref="G2:G10" si="0">IF(F2&lt;2,0,IF(F2&lt;6,1/12*F2-1/6,IF(F2&lt;15,1/27*F2+1/9,IF(F2&lt;=30,1/45*F2+1/3,1))))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="H2" s="2">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2:I10" si="1">IF(H2&lt;2,0,IF(H2&lt;9,1/14*H2-1/7,IF(H2&lt;30,1/42*H2+2/7,1)))</f>
+        <v>0.59523809523809523</v>
+      </c>
+      <c r="J2" s="2">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3">
+        <f>1/18*J2-1/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="L2" s="2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3">
+        <f>1/20*L2</f>
+        <v>0.2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3">
+        <f>1/20*N2</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>1/40*P2</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3">
+        <f>IF(R2&lt;10,1024/1023*(1-2^(-R2)),1)</f>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T2" s="2">
+        <v>4</v>
+      </c>
+      <c r="U2" s="3">
+        <f>IF(T2&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-T2)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0.34443709893310992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5700</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E11" si="2">1/40*D3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F3" s="2">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K11" si="3">1/18*J3-1/9</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M11" si="4">1/20*L3</f>
+        <v>0.75</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" ref="O3:O11" si="5">1/20*N3</f>
+        <v>0.25</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q11" si="6">1/40*P3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S11" si="7">IF(R3&lt;10,1024/1023*(1-2^(-R3)),1)</f>
+        <v>0.75073313782991202</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" ref="U3:U11" si="8">IF(T3&lt;3,1/4*(1-SQRT(5))*(1-(1/2*(1+SQRT(5)))^(3-T3)),0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="V3" s="6">
+        <v>1.1811202225070987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4725</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="8"/>
+        <v>0.5817316552559979</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0.95311641287991355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7800</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="F5" s="2">
+        <v>27</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>17</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="4"/>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="8"/>
+        <v>0.42576772571264371</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0.8622932515650924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1560</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H6" s="2">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="J6" s="2">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>16</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="P6" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="6"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="6">
+        <v>0.33677718806349211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4500</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>24</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>19</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="N7" s="2">
+        <v>16</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="8"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="V7" s="6">
+        <v>0.93878600139645307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6150</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>9</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N8" s="2">
+        <v>10</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>9</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.99902248289345064</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="8"/>
+        <v>0.1909830056250526</v>
+      </c>
+      <c r="V8" s="6">
+        <v>0.93671765192861756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1728</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="1"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L9" s="2">
+        <v>8</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>10</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="T9" s="2">
+        <v>4</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="6">
+        <v>0.31089460375324679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1859</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="F10" s="2">
+        <v>29</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="H10" s="2">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="J10" s="2">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666652</v>
+      </c>
+      <c r="L10" s="2">
+        <v>8</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>16</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="P10" s="2">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>10</v>
+      </c>
+      <c r="U10" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0.49970376936507938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4800</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F11" s="2">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4">
+        <f>IF(F11&lt;2,0,IF(F11&lt;6,1/12*F11-1/6,IF(F11&lt;15,1/27*F11+1/9,IF(F11&lt;=30,1/45*F11+1/3,1))))</f>
+        <v>0.62962962962962954</v>
+      </c>
+      <c r="H11" s="2">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4">
+        <f>IF(H11&lt;2,0,IF(H11&lt;9,1/14*H11-1/7,IF(H11&lt;30,1/42*H11+2/7,1)))</f>
+        <v>0.80952380952380942</v>
+      </c>
+      <c r="J11" s="2">
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+      <c r="S11" s="3">
+        <f t="shared" si="7"/>
+        <v>0.50048875855327468</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="U11" s="3">
+        <f t="shared" si="8"/>
+        <v>0.67172032305602269</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0.64990553645513494</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>SUMPRODUCT(B15:B24,V2:V11)</f>
+        <v>4.8462212461406544</v>
+      </c>
+      <c r="F15">
+        <f>SUMPRODUCT(B15:B24,B2:B11)</f>
+        <v>24494</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>